<commit_message>
Error Check Code, AZ, MR WY data update.
Error Check Code, AZ, MR WY data update.
</commit_message>
<xml_diff>
--- a/Montana/WaterAllocation/MT_Allocation Schema Mapping to WaDE_QA.xlsx
+++ b/Montana/WaterAllocation/MT_Allocation Schema Mapping to WaDE_QA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\MappingStatesDataToWaDE2.0\Montana\WaterAllocation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A994884-950D-4B9A-AB04-DE270DB6EAAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D85B9C-4976-4C2B-8EB6-5139A03006A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="714" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="714" activeTab="6" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping Notes" sheetId="10" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="304">
   <si>
     <t>Name</t>
   </si>
@@ -2428,7 +2428,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7154D4B-C952-456C-B506-1C3DB2041E3D}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -3945,7 +3945,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4617,8 +4617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B91B1FF-D207-4871-B787-27544A9D3030}">
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:XFD32"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5782,8 +5782,8 @@
       <c r="D38" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="E38" s="24" t="s">
-        <v>253</v>
+      <c r="E38" s="24">
+        <v>0</v>
       </c>
       <c r="F38" s="24" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
MT wr error data update
MT wr error data update
</commit_message>
<xml_diff>
--- a/Montana/WaterAllocation/MT_Allocation Schema Mapping to WaDE_QA.xlsx
+++ b/Montana/WaterAllocation/MT_Allocation Schema Mapping to WaDE_QA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\MappingStatesDataToWaDE2.0\Montana\WaterAllocation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D85B9C-4976-4C2B-8EB6-5139A03006A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0A8643-4926-4EEB-ABB1-DF628BA76302}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="714" activeTab="6" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="714" activeTab="5" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping Notes" sheetId="10" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="305">
   <si>
     <t>Name</t>
   </si>
@@ -978,6 +978,9 @@
   <si>
     <t>Replaced all ';' in ALL_OWNERS filed with a ','.</t>
   </si>
+  <si>
+    <t>This is  DPL derived value.  We don't need to worry about this.</t>
+  </si>
 </sst>
 </file>
 
@@ -986,7 +989,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="36" x14ac:knownFonts="1">
+  <fonts count="37" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1248,6 +1251,14 @@
     </font>
     <font>
       <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1766,7 +1777,7 @@
     <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2068,6 +2079,36 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2428,7 +2469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7154D4B-C952-456C-B506-1C3DB2041E3D}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -2513,7 +2554,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3944,8 +3985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10E7F0DF-14BE-4BB8-BB6C-8815808B0B66}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4484,34 +4525,34 @@
         <v>169</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="24" x14ac:dyDescent="0.3">
-      <c r="A20" s="35" t="s">
+    <row r="20" spans="1:10" s="103" customFormat="1" ht="24" x14ac:dyDescent="0.3">
+      <c r="A20" s="103" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="104" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="37" t="s">
+      <c r="C20" s="105" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="E20" s="24" t="s">
+      <c r="D20" s="106" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="107" t="s">
         <v>281</v>
       </c>
-      <c r="F20" s="47" t="s">
-        <v>38</v>
-      </c>
-      <c r="G20" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="H20" s="85"/>
-      <c r="I20" s="84" t="s">
+      <c r="F20" s="108" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="109" t="s">
+        <v>38</v>
+      </c>
+      <c r="H20" s="110"/>
+      <c r="I20" s="111" t="s">
         <v>123</v>
       </c>
-      <c r="J20" s="88" t="s">
-        <v>160</v>
+      <c r="J20" s="112" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -4617,8 +4658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B91B1FF-D207-4871-B787-27544A9D3030}">
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>